<commit_message>
trial - fix appendix c table figure
</commit_message>
<xml_diff>
--- a/tables/habitat/AllTables.xlsx
+++ b/tables/habitat/AllTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\Sherry Zhai\Github\cdm-science\tables\habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C5C439-BE6F-4F42-8EFE-FAA70010A5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF66ECC4-7433-45D6-921B-2E2409F02A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26990" yWindow="4800" windowWidth="23040" windowHeight="11550" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
+    <workbookView xWindow="27460" yWindow="320" windowWidth="23040" windowHeight="19880" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_NPMR" sheetId="1" r:id="rId1"/>
@@ -917,9 +917,6 @@
     <t>1-12/2018</t>
   </si>
   <si>
-    <t>HCHB_longterm</t>
-  </si>
-  <si>
     <t>Shoot count (HCHB)</t>
   </si>
   <si>
@@ -978,15 +975,6 @@
   </si>
   <si>
     <t>$LC^{23}_{10}$</t>
-  </si>
-  <si>
-    <t>Historical&lt;br&gt;(Appendix)</t>
-  </si>
-  <si>
-    <t>HCHB_v1&lt;br&gt;(Appendix)</t>
-  </si>
-  <si>
-    <t>HCHB_v2&lt;br&gt;(Appendix)</t>
   </si>
   <si>
     <t xml:space="preserve">Kim et al. 2013; </t>
@@ -1402,7 +1390,19 @@
     <t>Habitat Suitability Index ($\Phi$) function figure</t>
   </si>
   <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_viability_salinity.png" width="20"/&gt;</t>
+    <t>Historical&lt;br&gt;(Appendix C)</t>
+  </si>
+  <si>
+    <t>HCHB_v1&lt;br&gt;(Appendix C)</t>
+  </si>
+  <si>
+    <t>HCHB_v2&lt;br&gt;(Appendix C)</t>
+  </si>
+  <si>
+    <t>HCHB_Gen II</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_viability_salinity.png" width="5"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +2016,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,13 +2040,13 @@
         <v>153</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>32</v>
@@ -2092,10 +2092,10 @@
         <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>159</v>
@@ -2104,7 +2104,7 @@
         <v>38</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>151</v>
@@ -2115,7 +2115,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>151</v>
@@ -2124,10 +2124,10 @@
         <v>151</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>151</v>
@@ -2138,16 +2138,16 @@
         <v>47</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>151</v>
@@ -2210,10 +2210,10 @@
         <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>160</v>
@@ -2233,7 +2233,7 @@
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>151</v>
@@ -2242,10 +2242,10 @@
         <v>161</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>151</v>
@@ -2256,16 +2256,16 @@
         <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>151</v>
@@ -2279,16 +2279,16 @@
         <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>151</v>
@@ -2328,19 +2328,19 @@
         <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>43</v>
@@ -2351,7 +2351,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>151</v>
@@ -2360,13 +2360,13 @@
         <v>151</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>70</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2374,22 +2374,22 @@
         <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2397,19 +2397,19 @@
         <v>44</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>151</v>
@@ -2420,16 +2420,16 @@
         <v>157</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>49</v>
@@ -2446,19 +2446,19 @@
         <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>55</v>
@@ -2469,13 +2469,13 @@
         <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>151</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>172</v>
@@ -2492,16 +2492,16 @@
         <v>47</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>151</v>
@@ -2515,16 +2515,16 @@
         <v>44</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>151</v>
@@ -2538,13 +2538,13 @@
         <v>157</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>175</v>
@@ -2564,16 +2564,16 @@
         <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>160</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>151</v>
@@ -2587,7 +2587,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>151</v>
@@ -2602,7 +2602,7 @@
         <v>67</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2610,16 +2610,16 @@
         <v>47</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>151</v>
@@ -2633,16 +2633,16 @@
         <v>44</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>151</v>
@@ -2804,15 +2804,15 @@
         <v>185</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>186</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>186</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>186</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>194</v>
@@ -2892,7 +2892,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>187</v>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>187</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>187</v>
@@ -2952,7 +2952,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>187</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>220</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>222</v>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>222</v>
@@ -3053,24 +3053,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
         <v>241</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>242</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>243</v>
-      </c>
-      <c r="E1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B2">
         <v>64</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3">
         <v>73</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4">
         <v>85</v>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5">
         <v>88</v>
@@ -3138,13 +3138,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6">
         <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D6">
         <v>84</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B8">
         <v>108</v>
@@ -4119,7 +4119,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>311</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>219</v>
@@ -4195,7 +4195,7 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>312</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>148</v>
@@ -4224,7 +4224,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>313</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>148</v>
@@ -4253,7 +4253,7 @@
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>314</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>218</v>

</xml_diff>

<commit_message>
another try on fixing table
</commit_message>
<xml_diff>
--- a/tables/habitat/AllTables.xlsx
+++ b/tables/habitat/AllTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\Sherry Zhai\Github\cdm-science\tables\habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF66ECC4-7433-45D6-921B-2E2409F02A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED7C98A-440A-4340-B99B-4872EF03892F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27460" yWindow="320" windowWidth="23040" windowHeight="19880" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
   </bookViews>
@@ -704,15 +704,6 @@
     <t>Seed germination (Apr 1 – Jun 30)</t>
   </si>
   <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_germination_salinity.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_turion_salinity.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_turion_depth.png"&gt;</t>
-  </si>
-  <si>
     <t>&lt; 10 % of time wet: unsuitable&lt;br&gt;
 &gt;= 10 % of time wet: suitable&lt;br&gt;</t>
   </si>
@@ -1030,42 +1021,6 @@
   </si>
   <si>
     <t>Highest densities of turions were observed in 0.1–0.4 m water depths. However this depth preference is likely the result of trade-off between light requirement (thresholds included in $\Phi^{tur}_{L}$)) for photosynthesis and preventing desiccation</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_adult_temp.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_germination_temp.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_turion_temp.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_turion_light.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_adult_salinity.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_adult_light.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_adult_algae.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_flower_salinity.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_flower_depth.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_flower_temp.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_flower_light.png"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_flower_algae.png"&gt;</t>
   </si>
   <si>
     <t>$\Phi^{germ}_{S}$= 
@@ -1390,6 +1345,9 @@
     <t>Habitat Suitability Index ($\Phi$) function figure</t>
   </si>
   <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_viability_salinity.png" width="20"/&gt;</t>
+  </si>
+  <si>
     <t>Historical&lt;br&gt;(Appendix C)</t>
   </si>
   <si>
@@ -1402,7 +1360,49 @@
     <t>HCHB_Gen II</t>
   </si>
   <si>
-    <t>&lt;img src="images/lagoon_habitat/HSI_viability_salinity.png" width="5"/&gt;</t>
+    <t>&lt;img src="images/lagoon_habitat/HSI_germination_salinity.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_germination_temp.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_turion_temp.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_turion_salinity.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_turion_light.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_turion_depth.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_adult_salinity.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_adult_temp.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_adult_light.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_adult_algae.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_flower_salinity.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_flower_depth.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_flower_temp.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_flower_light.png" width="20"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="images/lagoon_habitat/HSI_flower_algae.png" width="20"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +2016,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,13 +2040,13 @@
         <v>153</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>32</v>
@@ -2072,7 +2072,7 @@
         <v>156</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>37</v>
@@ -2092,19 +2092,19 @@
         <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>159</v>
+        <v>301</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>151</v>
@@ -2115,7 +2115,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>151</v>
@@ -2124,10 +2124,10 @@
         <v>151</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>151</v>
@@ -2138,16 +2138,16 @@
         <v>47</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>151</v>
@@ -2210,13 +2210,13 @@
         <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>160</v>
+        <v>304</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>40</v>
@@ -2233,19 +2233,19 @@
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>151</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>161</v>
+        <v>306</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>151</v>
@@ -2256,16 +2256,16 @@
         <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>261</v>
+        <v>303</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>151</v>
@@ -2279,16 +2279,16 @@
         <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>262</v>
+        <v>305</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>151</v>
@@ -2320,7 +2320,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>51</v>
       </c>
@@ -2328,19 +2328,19 @@
         <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>263</v>
+        <v>307</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>43</v>
@@ -2351,7 +2351,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>151</v>
@@ -2360,13 +2360,13 @@
         <v>151</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>70</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2374,22 +2374,22 @@
         <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>259</v>
+        <v>308</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2397,19 +2397,19 @@
         <v>44</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>264</v>
+        <v>309</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>151</v>
@@ -2420,16 +2420,16 @@
         <v>157</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>265</v>
+        <v>310</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>49</v>
@@ -2446,19 +2446,19 @@
         <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>55</v>
@@ -2469,16 +2469,16 @@
         <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>151</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>267</v>
+        <v>312</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>66</v>
@@ -2492,16 +2492,16 @@
         <v>47</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>151</v>
@@ -2515,16 +2515,16 @@
         <v>44</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>269</v>
+        <v>314</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>151</v>
@@ -2538,16 +2538,16 @@
         <v>157</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>49</v>
@@ -2564,16 +2564,16 @@
         <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>160</v>
+        <v>304</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>151</v>
@@ -2587,7 +2587,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>151</v>
@@ -2596,13 +2596,13 @@
         <v>151</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>67</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2610,16 +2610,16 @@
         <v>47</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>261</v>
+        <v>303</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>151</v>
@@ -2633,16 +2633,16 @@
         <v>44</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>262</v>
+        <v>305</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>151</v>
@@ -2698,72 +2698,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2792,36 +2792,36 @@
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>185</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E2" s="2">
         <v>0.55000000000000004</v>
@@ -2832,16 +2832,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>189</v>
       </c>
       <c r="E3" s="2">
         <v>0.49</v>
@@ -2852,16 +2852,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>189</v>
       </c>
       <c r="E4" s="2">
         <v>0.25</v>
@@ -2872,16 +2872,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E5" s="2">
         <v>0.31</v>
@@ -2892,16 +2892,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E6" s="2">
         <v>3.4000000000000002E-2</v>
@@ -2912,16 +2912,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E7" s="2">
         <v>-0.13</v>
@@ -2932,16 +2932,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E8" s="2">
         <v>5.5E-2</v>
@@ -2952,16 +2952,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -2972,16 +2972,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E10" s="2">
         <v>-0.51</v>
@@ -2992,16 +2992,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E11" s="2">
         <v>0.25</v>
@@ -3012,16 +3012,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E12" s="2">
         <v>0.21</v>
@@ -3053,24 +3053,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" t="s">
         <v>240</v>
-      </c>
-      <c r="C1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B2">
         <v>64</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B3">
         <v>73</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B4">
         <v>85</v>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B5">
         <v>88</v>
@@ -3138,13 +3138,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B6">
         <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D6">
         <v>84</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B8">
         <v>108</v>
@@ -3434,7 +3434,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>75</v>
@@ -3446,7 +3446,7 @@
         <v>68</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.25">
@@ -3454,7 +3454,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>59</v>
@@ -3474,7 +3474,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>60</v>
@@ -3494,7 +3494,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>61</v>
@@ -3511,24 +3511,24 @@
     </row>
     <row r="6" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>70</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>62</v>
@@ -3545,13 +3545,13 @@
     </row>
     <row r="8" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>74</v>
@@ -3562,13 +3562,13 @@
     </row>
     <row r="9" spans="1:6" ht="201.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>49</v>
@@ -3582,7 +3582,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>72</v>
@@ -3599,13 +3599,13 @@
     </row>
     <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>66</v>
@@ -3616,13 +3616,13 @@
     </row>
     <row r="12" spans="1:6" ht="189" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>49</v>
@@ -3636,13 +3636,13 @@
         <v>57</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>94</v>
@@ -3653,19 +3653,19 @@
     </row>
     <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3872,7 +3872,7 @@
         <v>125</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>130</v>
@@ -3892,7 +3892,7 @@
         <v>126</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>130</v>
@@ -3932,7 +3932,7 @@
         <v>128</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>130</v>
@@ -4019,7 +4019,7 @@
         <v>150</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>151</v>
@@ -4036,10 +4036,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>62</v>
@@ -4056,10 +4056,10 @@
         <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>62</v>
@@ -4079,7 +4079,7 @@
         <v>64</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>62</v>
@@ -4096,10 +4096,10 @@
         <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>62</v>
@@ -4166,22 +4166,22 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
         <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G2" t="s">
         <v>143</v>
@@ -4195,7 +4195,7 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>148</v>
@@ -4204,13 +4204,13 @@
         <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G3" t="s">
         <v>143</v>
@@ -4224,7 +4224,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>148</v>
@@ -4233,13 +4233,13 @@
         <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" t="s">
         <v>213</v>
-      </c>
-      <c r="F4" t="s">
-        <v>216</v>
       </c>
       <c r="G4" t="s">
         <v>146</v>
@@ -4253,22 +4253,22 @@
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C5" t="s">
         <v>147</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5" t="s">
         <v>214</v>
-      </c>
-      <c r="F5" t="s">
-        <v>217</v>
       </c>
       <c r="G5" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
try citing in table
</commit_message>
<xml_diff>
--- a/tables/habitat/AllTables.xlsx
+++ b/tables/habitat/AllTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\Sherry Zhai\Github\cdm-science\tables\habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F99604-61CC-4335-A508-C3515B2CC9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22612521-6D78-4FF2-89D2-47BA3D82AB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27460" yWindow="3450" windowWidth="23040" windowHeight="16750" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_NPMR" sheetId="1" r:id="rId1"/>
@@ -968,9 +968,6 @@
     <t>$LC^{23}_{10}$</t>
   </si>
   <si>
-    <t xml:space="preserve">Kim et al. 2013; </t>
-  </si>
-  <si>
     <t>Assumed to be the same as adult growth</t>
   </si>
   <si>
@@ -1403,6 +1400,9 @@
   </si>
   <si>
     <t>&lt;img src="images/lagoon_habitat/HSI_flower_algae.png" width="160"/&gt;</t>
+  </si>
+  <si>
+    <t>\@kim2013</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +2016,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,13 +2040,13 @@
         <v>153</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>294</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>295</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>32</v>
@@ -2072,7 +2072,7 @@
         <v>156</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>37</v>
@@ -2092,19 +2092,19 @@
         <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>241</v>
+        <v>315</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>151</v>
@@ -2115,7 +2115,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>151</v>
@@ -2124,10 +2124,10 @@
         <v>151</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>151</v>
@@ -2138,16 +2138,16 @@
         <v>47</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>151</v>
@@ -2210,13 +2210,13 @@
         <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>40</v>
@@ -2233,19 +2233,19 @@
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>151</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>245</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>151</v>
@@ -2256,16 +2256,16 @@
         <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>151</v>
@@ -2279,16 +2279,16 @@
         <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>151</v>
@@ -2320,7 +2320,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>51</v>
       </c>
@@ -2328,19 +2328,19 @@
         <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>43</v>
@@ -2351,7 +2351,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>151</v>
@@ -2360,13 +2360,13 @@
         <v>151</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>70</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2374,22 +2374,22 @@
         <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F15" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2397,19 +2397,19 @@
         <v>44</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>151</v>
@@ -2420,16 +2420,16 @@
         <v>157</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>49</v>
@@ -2446,19 +2446,19 @@
         <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>55</v>
@@ -2469,13 +2469,13 @@
         <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>151</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>169</v>
@@ -2492,16 +2492,16 @@
         <v>47</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>151</v>
@@ -2515,16 +2515,16 @@
         <v>44</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>151</v>
@@ -2538,13 +2538,13 @@
         <v>157</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>172</v>
@@ -2564,16 +2564,16 @@
         <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>151</v>
@@ -2587,7 +2587,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>151</v>
@@ -2602,7 +2602,7 @@
         <v>67</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2610,16 +2610,16 @@
         <v>47</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>151</v>
@@ -2633,16 +2633,16 @@
         <v>44</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>151</v>
@@ -2804,10 +2804,10 @@
         <v>182</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3651,7 +3651,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>163</v>
       </c>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>216</v>
@@ -4195,7 +4195,7 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>148</v>
@@ -4224,7 +4224,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>148</v>
@@ -4253,7 +4253,7 @@
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
second try citing in table
</commit_message>
<xml_diff>
--- a/tables/habitat/AllTables.xlsx
+++ b/tables/habitat/AllTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\Sherry Zhai\Github\cdm-science\tables\habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22612521-6D78-4FF2-89D2-47BA3D82AB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95931AE1-E971-44ED-9E3D-E122F27C443A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="317">
   <si>
     <t>Field data</t>
   </si>
@@ -1402,7 +1402,11 @@
     <t>&lt;img src="images/lagoon_habitat/HSI_flower_algae.png" width="160"/&gt;</t>
   </si>
   <si>
-    <t>\@kim2013</t>
+    <t>\"@kim2013"</t>
+  </si>
+  <si>
+    <t>"@kim2013";&lt;br&gt;
+Kim et al. 2015</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +2020,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,7 +2082,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>68</v>
+        <v>316</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
another try at ref in table
</commit_message>
<xml_diff>
--- a/tables/habitat/AllTables.xlsx
+++ b/tables/habitat/AllTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\Sherry Zhai\Github\cdm-science\tables\habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B09D94-370E-475F-8F89-267D07F9390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD22302-80B4-4107-B92B-5C6103160C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44690" yWindow="-6100" windowWidth="38620" windowHeight="21220" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="870" firstSheet="3" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_NPMR" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="321">
   <si>
     <t>Field data</t>
   </si>
@@ -167,18 +167,10 @@
 In salinity below 40g/L a germination probability of &gt;50% would be expected for seeds of R. tuberosa, but at salinities between 40 and 90 g/L germination would be&lt;50%</t>
   </si>
   <si>
-    <t>Kim et al. 2013</t>
-  </si>
-  <si>
     <t>Turions of R. tuberosa germinated at salinities of 0 to 125g/L, with 14 - 74% germination, but no germination occurred above 125 g/L. Suboptimal thresholds based on Fig.2 in Kim et al. 2013</t>
   </si>
   <si>
     <t>D: Water depth (m)</t>
-  </si>
-  <si>
-    <t>A primary factor driving the distribution and abundance of Ruppia in the southern Coorong. The highest abundance of R. tuberosa found at salinities from 19 to 70 g/L and declined sharply
-in response to increasing salinity from 70 to 109 g/L, but increased again between 116 and 124 g/L.
-Table 2 in Collier et al. 2017 indicated R. tuberosa occurred at up to 230 g/L in other Lakes but source of data is not clear. Lower threshold source based on Fig.5 in Asanopoulos &amp; Waycott 2020</t>
   </si>
   <si>
     <t>The model relating shoot density to physicochemical
@@ -192,19 +184,12 @@
 weeks of shading. Biomass was significantly reduced in the 5% light treatment compared to the 36, 63, 86 and 100% light treatment.</t>
   </si>
   <si>
-    <t>Collier et al. 2017
-cited in Asanopoulos &amp; Waycott 2020</t>
-  </si>
-  <si>
     <t>T: Temperature (°C)</t>
   </si>
   <si>
     <t>The optimum is not specifically for R. tuberosa.</t>
   </si>
   <si>
-    <t>Lewis et al. 2022</t>
-  </si>
-  <si>
     <t>Flowering and seed set (Sep 1 – Dec 31)</t>
   </si>
   <si>
@@ -215,12 +200,6 @@
   </si>
   <si>
     <t>Seed germination  (Apr 1 – Jun 30)</t>
-  </si>
-  <si>
-    <t>Flower abundance was highest at salinities between ~47 and 62 g/L and flower abundance was lowest at &gt;70 g/L and &lt;47 g/L.
-The highest seed density was maintained at salinities of
-26–62 g/L.
-Upper and lower thresholds were based on Collier et al. 2017 and Fig.5 in Asanopoulos &amp; Waycott 2020. Original source unclear</t>
   </si>
   <si>
     <t>The model relating flower density to physicochemical
@@ -279,27 +258,6 @@
 &gt;230 unsuitable</t>
   </si>
   <si>
-    <t>Kim et al. 2015;&lt;br&gt;
-Collier et al. 2017;</t>
-  </si>
-  <si>
-    <t>Kim et al. 2015;&lt;br&gt;
-Collier et al. 2017;&lt;br&gt;
-Asanopoulos &amp; Waycott 2020</t>
-  </si>
-  <si>
-    <t>Kim et al. 2013;&lt;br&gt;
-Kim et al. 2015</t>
-  </si>
-  <si>
-    <t>Kim et al. 2013;&lt;br&gt;
-Asanopoulos &amp; Waycott 2020 Fig.5</t>
-  </si>
-  <si>
-    <t>Kim et al. 2015;&lt;br&gt;
-Collier et al. 2017</t>
-  </si>
-  <si>
     <t>&lt;=100 optimal&lt;br&gt;
 100-368 suboptimal&lt;br&gt;
 &gt;368 unsuitable</t>
@@ -310,15 +268,6 @@
 47-62 optimal&lt;br&gt;
 62-100 suboptimal&lt;br&gt;
 &gt;100 unsuitable</t>
-  </si>
-  <si>
-    <t>Brock 1982;&lt;br&gt; Kim et al. 2015;&lt;br&gt;
-Collier et al. 2017;&lt;br&gt;
-Asanopoulos &amp; Waycott 2020</t>
-  </si>
-  <si>
-    <t>Santamaria &amp;
-Hootsmans 1998 cited in Collier et al. 2017.</t>
   </si>
   <si>
     <t>&lt;135 optimal&lt;br&gt;
@@ -437,10 +386,6 @@
 salinity,&lt;br&gt;
 elevation,&lt;br&gt;
 distance from Murray Mouth</t>
-  </si>
-  <si>
-    <t>1. Kim et al. 2015;&lt;br&gt;
-3. Asanopoulos &amp; Waycott 2020</t>
   </si>
   <si>
     <t>Seed count&lt;br&gt; (R. tuberosa)</t>
@@ -736,9 +681,6 @@
     <t xml:space="preserve">Highest densities of turions were observed in 0.1–0.4 m water depths. However this depth preference is likely the result of trade-off between light requirement (thresholds included in f(l)) for photosynthesis and preventing desiccation. </t>
   </si>
   <si>
-    <t>R. tuberosa flowers need to reach the water surface for pollination. The highest density of flowering has been observed in water depths from 0.1 to 0.4 m and seed density of mature plants declines at depths greater than 0.4 m. Upper thresholds based on Fig.4 in Kim et al. 2015.</t>
-  </si>
-  <si>
     <t>&lt;0.01 unsuitable&lt;br&gt;
 0.01-0.1 suboptimal&lt;br&gt;
 0.1-0.4 optimal&lt;br&gt;
@@ -752,12 +694,6 @@
     <t>Surface mats formed
 by the filamentous algae shade submerged plants and entangle flowers/fruits, causing them to break away from stems before they mature. 
 It was suggested that to maintain and improve the condition and resilience of the Ruppia community, algal mat formation should be reduced to less than 100 g/DW per m2. Upper thresholds derived from analysis of HCHB survey data (Figure 8.9)</t>
-  </si>
-  <si>
-    <t>Thresholds were determined considering several sources:
-1) The highest turion densities in the Coorong have been observed at salinity between ~124 g/L and 160 g/L and are most likely to occur where salinities are over 70 g/L. This study was conducted during a year with extremely high salinities in the Coorong;
-2) Analysis of 2020 – 2021 HCHB survey data indicates high turion abundance between ~70 – 120 g/L but can occur in salinity at as low as ~40g/L (Figure 8.6);
-3) Upper threshold based on Fig.5 in Asanopoulos &amp; Waycott 2020</t>
   </si>
   <si>
     <t>Surface mats formed
@@ -1383,10 +1319,6 @@
 \@collier2017</t>
   </si>
   <si>
-    <t>Santamarı́a &amp;
-Hootsmans 1998 cited in \@collier2017.</t>
-  </si>
-  <si>
     <t>\@collier2017 
 cited in \@asano2020</t>
   </si>
@@ -1414,6 +1346,11 @@
   <si>
     <t>The model relating shoot density to physicochemical
 conditions explained 73% of variation \[@kim2015]</t>
+  </si>
+  <si>
+    <t>A primary factor driving the distribution and abundance of Ruppia in the southern Coorong. The highest abundance of R. tuberosa found at salinities from 19 to 70 g/L and declined sharply
+in response to increasing salinity from 70 to 109 g/L, but increased again between 116 and 124 g/L.
+Table 2 in Collier et al. 2017 indicated R. tuberosa occurred at up to 230 g/L in other Lakes but source of data is not clear. Lower threshold source based on Fig.5 in \@asano2020</t>
   </si>
   <si>
     <t>A primary factor driving the distribution and abundance of Ruppia in the southern Coorong. The highest abundance of R. tuberosa found at salinities from 19 to 70 g/L and declined sharply
@@ -1443,6 +1380,46 @@
     <t>\@brock1982; &lt;br&gt;\@kim2015;&lt;br&gt;
 \@collier2017; &lt;br&gt;
 \@asano2020</t>
+  </si>
+  <si>
+    <t>1. \@kim2015;&lt;br&gt;
+3. \@asano2020</t>
+  </si>
+  <si>
+    <t>Thresholds were determined considering several sources:
+1) The highest turion densities in the Coorong have been observed at salinity between ~124 g/L and 160 g/L and are most likely to occur where salinities are over 70 g/L. This study was conducted during a year with extremely high salinities in the Coorong;
+2) Analysis of 2020 – 2021 HCHB survey data indicates high turion abundance between ~70 – 120 g/L but can occur in salinity at as low as ~40g/L (Figure 8.6);
+3) Upper threshold based on Fig.5 in \@asano2020</t>
+  </si>
+  <si>
+    <t>R. tuberosa flowers need to reach the water surface for pollination. The highest density of flowering has been observed in water depths from 0.1 to 0.4 m and seed density of mature plants declines at depths greater than 0.4 m. Upper thresholds based on Fig.4 in\@kim2015.</t>
+  </si>
+  <si>
+    <t>Flower abundance was highest at salinities between ~47 and 62 g/L and flower abundance was lowest at &gt;70 g/L and &lt;47 g/L.
+The highest seed density was maintained at salinities of
+26–62 g/L.
+Upper and lower thresholds were based on Collier et al. 2017 and Fig.5 in \@asano2020. Original source unclear</t>
+  </si>
+  <si>
+    <t>\@kim2015;&lt;br&gt;
+\@asano2020</t>
+  </si>
+  <si>
+    <t>Turions of R. tuberosa germinated at salinities of 0 to 125g/L, with 14 - 74% germination, but no germination occurred above 125 g/L. Suboptimal thresholds based on Fig.2 in\@kim2013</t>
+  </si>
+  <si>
+    <t>\@santa1998 cited in \@collier2017.</t>
+  </si>
+  <si>
+    <t>\"@kim2013";&lt;br&gt;
+"\@kim2015"</t>
+  </si>
+  <si>
+    <t>"@kim2013"</t>
+  </si>
+  <si>
+    <t>&lt;@kim2013&gt;;&lt;br&gt;
+\@asano2020 Fig.5</t>
   </si>
 </sst>
 </file>
@@ -1868,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1885,10 +1862,10 @@
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2">
         <v>0.72199999999999998</v>
@@ -1908,10 +1885,10 @@
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2">
         <v>0.25</v>
@@ -1931,10 +1908,10 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2">
         <v>0.95399999999999996</v>
@@ -1954,10 +1931,10 @@
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2">
         <v>0.27500000000000002</v>
@@ -1977,10 +1954,10 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2">
         <v>0.26400000000000001</v>
@@ -2003,7 +1980,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2">
         <v>0.44</v>
@@ -2026,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2">
         <v>0.54900000000000004</v>
@@ -2055,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E455835C-91A3-4A35-A210-9F3EF1BB69F6}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,19 +2051,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>32</v>
@@ -2106,612 +2083,612 @@
         <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="E17" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>318</v>
-      </c>
       <c r="H17" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>151</v>
+        <v>309</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>315</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2738,72 +2715,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2832,36 +2809,36 @@
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="E2" s="2">
         <v>0.55000000000000004</v>
@@ -2872,16 +2849,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="E3" s="2">
         <v>0.49</v>
@@ -2892,16 +2869,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="E4" s="2">
         <v>0.25</v>
@@ -2912,16 +2889,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="E5" s="2">
         <v>0.31</v>
@@ -2932,16 +2909,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="E6" s="2">
         <v>3.4000000000000002E-2</v>
@@ -2952,16 +2929,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E7" s="2">
         <v>-0.13</v>
@@ -2972,16 +2949,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E8" s="2">
         <v>5.5E-2</v>
@@ -2992,16 +2969,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -3012,16 +2989,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="E10" s="2">
         <v>-0.51</v>
@@ -3032,16 +3009,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="E11" s="2">
         <v>0.25</v>
@@ -3052,16 +3029,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="E12" s="2">
         <v>0.21</v>
@@ -3093,24 +3070,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B2">
         <v>64</v>
@@ -3127,7 +3104,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B3">
         <v>73</v>
@@ -3144,7 +3121,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B4">
         <v>85</v>
@@ -3161,7 +3138,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="B5">
         <v>88</v>
@@ -3178,13 +3155,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B6">
         <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D6">
         <v>84</v>
@@ -3195,7 +3172,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -3212,7 +3189,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="B8">
         <v>108</v>
@@ -3268,7 +3245,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
@@ -3282,7 +3259,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>23</v>
@@ -3310,7 +3287,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
@@ -3324,13 +3301,13 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3338,7 +3315,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
@@ -3388,13 +3365,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -3402,7 +3379,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>27</v>
@@ -3416,7 +3393,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>28</v>
@@ -3434,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A7A0F3-CFE1-4E54-A6CA-9E246D862933}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,238 +3451,238 @@
         <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>68</v>
+      <c r="E2" s="7" t="s">
+        <v>301</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>39</v>
+      <c r="E3" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>69</v>
+        <v>316</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>295</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="224.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>70</v>
+        <v>148</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>161</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>317</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="201.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>49</v>
+        <v>159</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>302</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>66</v>
+        <v>313</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>299</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="189" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>49</v>
+        <v>158</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>302</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>67</v>
+        <v>157</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>300</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3730,44 +3707,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3791,53 +3768,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3869,119 +3846,119 @@
         <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4013,139 +3990,139 @@
         <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4177,147 +4154,147 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="G1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="H1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="G2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="H2">
         <v>600</v>
       </c>
       <c r="I2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="G3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="H3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="I3" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="G4" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="H4">
         <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="F5" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="G5" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="H5">
         <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update habitat and renv.lock
</commit_message>
<xml_diff>
--- a/tables/habitat/AllTables.xlsx
+++ b/tables/habitat/AllTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\Sherry Zhai\Github\cdm-science\tables\habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48421F59-99E5-4D50-B157-B86039E4C291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D73E59-3D22-4333-A175-D0B5D1E1CC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27460" yWindow="320" windowWidth="23040" windowHeight="19880" tabRatio="870" firstSheet="5" activeTab="9" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
+    <workbookView xWindow="3420" yWindow="2715" windowWidth="32175" windowHeight="15435" tabRatio="870" activeTab="8" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_NPMR" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Sheet11_valid_hist" sheetId="12" r:id="rId11"/>
     <sheet name="Sheet12_valid_hchb" sheetId="11" r:id="rId12"/>
     <sheet name="Sheet13_fishtolerance" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet14_valid_hchbv2.1" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="328">
   <si>
     <t>Field data</t>
   </si>
@@ -575,9 +576,6 @@
   </si>
   <si>
     <t>tailored</t>
-  </si>
-  <si>
-    <t>Gen II</t>
   </si>
   <si>
     <t>HCHB&lt;br&gt;(Sep 2020 – Apr 2021)</t>
@@ -805,22 +803,10 @@
     <t>Gen 0&lt;br&gt; (Table 8.6)</t>
   </si>
   <si>
-    <t>Gen II&lt;br&gt; (Table 8.8)</t>
-  </si>
-  <si>
     <t>Gen 0&lt;br&gt; (Table 8.5)</t>
   </si>
   <si>
-    <t>Gen II&lt;br&gt; (Table 8.7)</t>
-  </si>
-  <si>
     <t>Gen 0&lt;br&gt; (Eq.8.5 - 8.6)</t>
-  </si>
-  <si>
-    <t>Gen II&lt;br&gt; (Eq.8.7 - 8.8)*</t>
-  </si>
-  <si>
-    <t>Gen II&lt;br&gt; (Eq.8.7 - 8.8)</t>
   </si>
   <si>
     <t xml:space="preserve">HCHB&lt;br&gt;(Sep 2020 – Dec 2021);&lt;br&gt; MDBA (2018 - 2019) </t>
@@ -1227,12 +1213,6 @@
 &gt;= 10 % of time wet: suitable</t>
   </si>
   <si>
-    <t>R&lt;br&gt;(Whole lagoon)</t>
-  </si>
-  <si>
-    <t>R&lt;br&gt;(South lagoon)</t>
-  </si>
-  <si>
     <t>Threshold</t>
   </si>
   <si>
@@ -1249,9 +1229,6 @@
   </si>
   <si>
     <t>HCHB_v2&lt;br&gt;(Appendix C)</t>
-  </si>
-  <si>
-    <t>HCHB_Gen II</t>
   </si>
   <si>
     <t>&lt;img src="images/lagoon_habitat/HSI_viability_salinity.png" width="160"/&gt;</t>
@@ -1412,6 +1389,57 @@
   </si>
   <si>
     <t>@collier2017</t>
+  </si>
+  <si>
+    <t>rs&lt;br&gt;(Whole lagoon)</t>
+  </si>
+  <si>
+    <t>rs&lt;br&gt;(South lagoon)</t>
+  </si>
+  <si>
+    <t>fit&lt;br&gt;(Whole lagoon)</t>
+  </si>
+  <si>
+    <t>fit&lt;br&gt;(South lagoon)</t>
+  </si>
+  <si>
+    <t>score&lt;br&gt;(Whole lagoon)</t>
+  </si>
+  <si>
+    <t>score&lt;br&gt;(South lagoon)</t>
+  </si>
+  <si>
+    <t>HCHB_Gen 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCHB&lt;br&gt;(Sep 2020 – Dec 2021) </t>
+  </si>
+  <si>
+    <t>Gen 2.1</t>
+  </si>
+  <si>
+    <t>r&lt;br&gt;(Whole lagoon)</t>
+  </si>
+  <si>
+    <t>r&lt;br&gt;(South lagoon)</t>
+  </si>
+  <si>
+    <t>HCHB_Gen 2.0&lt;br&gt;(Appendix C)</t>
+  </si>
+  <si>
+    <t>Gen 2.0</t>
+  </si>
+  <si>
+    <t>Gen 2.0&lt;br&gt; (Table 8.8)</t>
+  </si>
+  <si>
+    <t>Gen 2.0&lt;br&gt; (Table 8.7)</t>
+  </si>
+  <si>
+    <t>Gen 2.0&lt;br&gt; (Eq.8.7 - 8.8)*</t>
+  </si>
+  <si>
+    <t>Gen 2.0&lt;br&gt; (Eq.8.7 - 8.8)</t>
   </si>
 </sst>
 </file>
@@ -2030,7 +2058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E455835C-91A3-4A35-A210-9F3EF1BB69F6}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -2049,19 +2077,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>32</v>
@@ -2081,48 +2109,48 @@
         <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2130,22 +2158,22 @@
         <v>39</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2153,22 +2181,22 @@
         <v>43</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2176,45 +2204,45 @@
         <v>41</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2225,22 +2253,22 @@
         <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2248,22 +2276,22 @@
         <v>39</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2271,22 +2299,22 @@
         <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2294,45 +2322,45 @@
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2343,22 +2371,22 @@
         <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="240" x14ac:dyDescent="0.25">
@@ -2366,22 +2394,22 @@
         <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2389,22 +2417,22 @@
         <v>43</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2412,45 +2440,45 @@
         <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2461,22 +2489,22 @@
         <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -2484,19 +2512,19 @@
         <v>39</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>50</v>
@@ -2507,22 +2535,22 @@
         <v>43</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -2530,45 +2558,45 @@
         <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="225" x14ac:dyDescent="0.25">
@@ -2579,22 +2607,22 @@
         <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="210" x14ac:dyDescent="0.25">
@@ -2602,22 +2630,22 @@
         <v>39</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -2625,22 +2653,22 @@
         <v>43</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -2648,45 +2676,45 @@
         <v>41</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2713,72 +2741,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2791,7 +2819,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,36 +2835,36 @@
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>166</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>267</v>
+        <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>268</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E2" s="2">
         <v>0.55000000000000004</v>
@@ -2847,16 +2875,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="E3" s="2">
         <v>0.49</v>
@@ -2867,16 +2895,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" s="2">
         <v>0.25</v>
@@ -2887,16 +2915,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>176</v>
       </c>
       <c r="E5" s="2">
         <v>0.31</v>
@@ -2907,16 +2935,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" s="2">
         <v>3.4000000000000002E-2</v>
@@ -2927,16 +2955,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="D7" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" s="2">
         <v>-0.13</v>
@@ -2947,16 +2975,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="D8" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="2">
         <v>5.5E-2</v>
@@ -2967,16 +2995,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -2987,16 +3015,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E10" s="2">
         <v>-0.51</v>
@@ -3007,16 +3035,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E11" s="2">
         <v>0.25</v>
@@ -3027,16 +3055,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E12" s="2">
         <v>0.21</v>
@@ -3068,24 +3096,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B2">
         <v>64</v>
@@ -3102,7 +3130,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B3">
         <v>73</v>
@@ -3119,7 +3147,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B4">
         <v>85</v>
@@ -3136,7 +3164,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B5">
         <v>88</v>
@@ -3153,13 +3181,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B6">
         <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D6">
         <v>84</v>
@@ -3170,7 +3198,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -3187,7 +3215,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B8">
         <v>108</v>
@@ -3205,6 +3233,350 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6839B937-9303-4D91-AA10-917C5E77A1BA}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="G2">
+        <v>0.66</v>
+      </c>
+      <c r="H2">
+        <v>0.69</v>
+      </c>
+      <c r="I2">
+        <v>1.41</v>
+      </c>
+      <c r="J2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="G3">
+        <v>0.82</v>
+      </c>
+      <c r="H3">
+        <v>0.86</v>
+      </c>
+      <c r="I3">
+        <v>2.69</v>
+      </c>
+      <c r="J3">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="G4">
+        <v>0.61</v>
+      </c>
+      <c r="H4">
+        <v>0.67</v>
+      </c>
+      <c r="I4">
+        <v>1.37</v>
+      </c>
+      <c r="J4">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="G5">
+        <v>0.61</v>
+      </c>
+      <c r="H5">
+        <v>0.6</v>
+      </c>
+      <c r="I5">
+        <v>1.38</v>
+      </c>
+      <c r="J5">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="G6">
+        <v>0.67</v>
+      </c>
+      <c r="H6">
+        <v>0.66</v>
+      </c>
+      <c r="I6">
+        <v>1.62</v>
+      </c>
+      <c r="J6">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="G7">
+        <v>0.47</v>
+      </c>
+      <c r="H7">
+        <v>0.39</v>
+      </c>
+      <c r="I7">
+        <v>0.89</v>
+      </c>
+      <c r="J7">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-4.2000000000000003E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.74</v>
+      </c>
+      <c r="H8">
+        <v>0.76</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="G9">
+        <v>0.72</v>
+      </c>
+      <c r="H9">
+        <v>0.77</v>
+      </c>
+      <c r="I9">
+        <v>0.89</v>
+      </c>
+      <c r="J9">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H10">
+        <v>0.48</v>
+      </c>
+      <c r="I10">
+        <v>1.52</v>
+      </c>
+      <c r="J10">
+        <v>1.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3449,7 +3821,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>62</v>
@@ -3458,10 +3830,10 @@
         <v>37</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.25">
@@ -3469,7 +3841,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>53</v>
@@ -3478,10 +3850,10 @@
         <v>38</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3489,19 +3861,19 @@
         <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="224.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3509,16 +3881,16 @@
         <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>40</v>
@@ -3526,24 +3898,24 @@
     </row>
     <row r="6" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>56</v>
@@ -3552,24 +3924,24 @@
         <v>42</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="E8" s="13" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>44</v>
@@ -3577,19 +3949,19 @@
     </row>
     <row r="9" spans="1:6" ht="201.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -3597,16 +3969,16 @@
         <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>49</v>
@@ -3614,16 +3986,16 @@
     </row>
     <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>50</v>
@@ -3631,19 +4003,19 @@
     </row>
     <row r="12" spans="1:6" ht="189" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="225" x14ac:dyDescent="0.25">
@@ -3651,16 +4023,16 @@
         <v>51</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>52</v>
@@ -3668,19 +4040,19 @@
     </row>
     <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3867,16 +4239,16 @@
         <v>110</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -3887,7 +4259,7 @@
         <v>111</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>116</v>
@@ -3896,7 +4268,7 @@
         <v>117</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -3907,7 +4279,7 @@
         <v>112</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>116</v>
@@ -3933,7 +4305,7 @@
         <v>116</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>118</v>
@@ -3947,16 +4319,16 @@
         <v>114</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4011,16 +4383,16 @@
         <v>62</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -4031,16 +4403,16 @@
         <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -4051,16 +4423,16 @@
         <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -4071,10 +4443,10 @@
         <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>56</v>
@@ -4094,7 +4466,7 @@
         <v>58</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>56</v>
@@ -4111,16 +4483,16 @@
         <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4131,15 +4503,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E1DF35-3470-4741-B035-2FAF41BF3870}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -4158,7 +4530,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D1" t="s">
         <v>122</v>
@@ -4181,22 +4553,22 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
         <v>128</v>
       </c>
       <c r="D2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" t="s">
         <v>192</v>
       </c>
-      <c r="E2" t="s">
-        <v>194</v>
-      </c>
       <c r="F2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G2" t="s">
         <v>129</v>
@@ -4210,22 +4582,22 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
         <v>128</v>
       </c>
       <c r="D3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" t="s">
         <v>192</v>
       </c>
-      <c r="E3" t="s">
-        <v>194</v>
-      </c>
       <c r="F3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G3" t="s">
         <v>129</v>
@@ -4239,22 +4611,22 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
         <v>128</v>
       </c>
       <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
         <v>192</v>
       </c>
-      <c r="E4" t="s">
-        <v>194</v>
-      </c>
       <c r="F4" t="s">
-        <v>197</v>
+        <v>326</v>
       </c>
       <c r="G4" t="s">
         <v>132</v>
@@ -4263,27 +4635,27 @@
         <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>322</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>323</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>324</v>
       </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>325</v>
       </c>
       <c r="F5" t="s">
-        <v>198</v>
+        <v>327</v>
       </c>
       <c r="G5" t="s">
         <v>132</v>
@@ -4292,7 +4664,36 @@
         <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E6" t="s">
+        <v>325</v>
+      </c>
+      <c r="F6" t="s">
+        <v>327</v>
+      </c>
+      <c r="G6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6">
+        <v>101</v>
+      </c>
+      <c r="I6" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Ruppia and Macroalgae chapters
</commit_message>
<xml_diff>
--- a/tables/habitat/AllTables.xlsx
+++ b/tables/habitat/AllTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\Sherry Zhai\Github\cdm-science\tables\habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D73E59-3D22-4333-A175-D0B5D1E1CC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A104FF7-F3F5-45FF-B177-8E1ADCC377EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2715" windowWidth="32175" windowHeight="15435" tabRatio="870" activeTab="8" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="870" activeTab="13" xr2:uid="{C6B6A4F7-8E11-4364-B90C-81D0188035FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_NPMR" sheetId="1" r:id="rId1"/>
@@ -1397,12 +1397,6 @@
     <t>rs&lt;br&gt;(South lagoon)</t>
   </si>
   <si>
-    <t>fit&lt;br&gt;(Whole lagoon)</t>
-  </si>
-  <si>
-    <t>fit&lt;br&gt;(South lagoon)</t>
-  </si>
-  <si>
     <t>score&lt;br&gt;(Whole lagoon)</t>
   </si>
   <si>
@@ -1440,6 +1434,12 @@
   </si>
   <si>
     <t>Gen 2.0&lt;br&gt; (Eq.8.7 - 8.8)</t>
+  </si>
+  <si>
+    <t>fit&lt;br&gt;(%, Whole lagoon)</t>
+  </si>
+  <si>
+    <t>fit&lt;br&gt;(%, South lagoon)</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1531,6 +1531,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2847,10 +2848,10 @@
         <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3240,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6839B937-9303-4D91-AA10-917C5E77A1BA}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3274,16 +3275,16 @@
         <v>312</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3299,23 +3300,23 @@
       <c r="D2" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E2" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="G2">
-        <v>0.66</v>
-      </c>
-      <c r="H2">
-        <v>0.69</v>
+      <c r="E2">
+        <v>0.53</v>
+      </c>
+      <c r="F2">
+        <v>0.4</v>
+      </c>
+      <c r="G2" s="15">
+        <v>68</v>
+      </c>
+      <c r="H2" s="15">
+        <v>69</v>
       </c>
       <c r="I2">
-        <v>1.41</v>
+        <v>1.37</v>
       </c>
       <c r="J2">
-        <v>1.5</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3331,23 +3332,23 @@
       <c r="D3" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.36</v>
-      </c>
-      <c r="G3">
-        <v>0.82</v>
-      </c>
-      <c r="H3">
-        <v>0.86</v>
+      <c r="E3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F3">
+        <v>0.38</v>
+      </c>
+      <c r="G3" s="15">
+        <v>80</v>
+      </c>
+      <c r="H3" s="15">
+        <v>81</v>
       </c>
       <c r="I3">
-        <v>2.69</v>
+        <v>2.48</v>
       </c>
       <c r="J3">
-        <v>3.54</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3363,23 +3364,23 @@
       <c r="D4" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.36</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.43</v>
-      </c>
-      <c r="G4">
-        <v>0.61</v>
-      </c>
-      <c r="H4">
-        <v>0.67</v>
+      <c r="E4">
+        <v>0.31</v>
+      </c>
+      <c r="F4">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="15">
+        <v>61</v>
+      </c>
+      <c r="H4" s="15">
+        <v>69</v>
       </c>
       <c r="I4">
-        <v>1.37</v>
+        <v>1.3</v>
       </c>
       <c r="J4">
-        <v>1.36</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3395,23 +3396,23 @@
       <c r="D5" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.44</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.44</v>
-      </c>
-      <c r="G5">
-        <v>0.61</v>
-      </c>
-      <c r="H5">
-        <v>0.6</v>
+      <c r="E5">
+        <v>0.41</v>
+      </c>
+      <c r="F5">
+        <v>0.37</v>
+      </c>
+      <c r="G5" s="15">
+        <v>57.999999999999993</v>
+      </c>
+      <c r="H5" s="15">
+        <v>56.999999999999993</v>
       </c>
       <c r="I5">
-        <v>1.38</v>
+        <v>1.24</v>
       </c>
       <c r="J5">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3427,23 +3428,23 @@
       <c r="D6" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
+        <v>0.37</v>
+      </c>
+      <c r="F6">
         <v>0.45</v>
       </c>
-      <c r="F6" s="2">
-        <v>0.52</v>
-      </c>
-      <c r="G6">
-        <v>0.67</v>
-      </c>
-      <c r="H6">
-        <v>0.66</v>
+      <c r="G6" s="15">
+        <v>66</v>
+      </c>
+      <c r="H6" s="15">
+        <v>66</v>
       </c>
       <c r="I6">
-        <v>1.62</v>
+        <v>1.43</v>
       </c>
       <c r="J6">
-        <v>1.85</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3459,23 +3460,23 @@
       <c r="D7" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.38</v>
-      </c>
-      <c r="G7">
-        <v>0.47</v>
-      </c>
-      <c r="H7">
-        <v>0.39</v>
+      <c r="E7">
+        <v>0.22</v>
+      </c>
+      <c r="F7">
+        <v>0.34</v>
+      </c>
+      <c r="G7" s="15">
+        <v>48</v>
+      </c>
+      <c r="H7" s="15">
+        <v>42</v>
       </c>
       <c r="I7">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="J7">
-        <v>0.72</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3491,17 +3492,17 @@
       <c r="D8" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E8" s="2">
-        <v>-6.2E-2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>-4.2000000000000003E-2</v>
-      </c>
-      <c r="G8">
-        <v>0.74</v>
-      </c>
-      <c r="H8">
-        <v>0.76</v>
+      <c r="E8">
+        <v>-0.13</v>
+      </c>
+      <c r="F8">
+        <v>-0.11</v>
+      </c>
+      <c r="G8" s="15">
+        <v>72</v>
+      </c>
+      <c r="H8" s="15">
+        <v>76</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -3523,20 +3524,20 @@
       <c r="D9" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E9" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="G9">
-        <v>0.72</v>
-      </c>
-      <c r="H9">
-        <v>0.77</v>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <v>0.11</v>
+      </c>
+      <c r="G9" s="15">
+        <v>74</v>
+      </c>
+      <c r="H9" s="15">
+        <v>77</v>
       </c>
       <c r="I9">
-        <v>0.89</v>
+        <v>1.24</v>
       </c>
       <c r="J9">
         <v>0.89</v>
@@ -3555,20 +3556,20 @@
       <c r="D10" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G10">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H10">
-        <v>0.48</v>
+      <c r="E10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F10">
+        <v>0.51</v>
+      </c>
+      <c r="G10" s="15">
+        <v>56.999999999999993</v>
+      </c>
+      <c r="H10" s="15">
+        <v>49</v>
       </c>
       <c r="I10">
-        <v>1.52</v>
+        <v>1.62</v>
       </c>
       <c r="J10">
         <v>1.01</v>
@@ -4505,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E1DF35-3470-4741-B035-2FAF41BF3870}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4626,7 +4627,7 @@
         <v>192</v>
       </c>
       <c r="F4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G4" t="s">
         <v>132</v>
@@ -4640,22 +4641,22 @@
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>194</v>
       </c>
       <c r="C5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E5" t="s">
         <v>323</v>
       </c>
-      <c r="D5" t="s">
-        <v>324</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>325</v>
-      </c>
-      <c r="F5" t="s">
-        <v>327</v>
       </c>
       <c r="G5" t="s">
         <v>132</v>
@@ -4669,28 +4670,28 @@
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" t="s">
         <v>317</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="C6" t="s">
-        <v>319</v>
-      </c>
       <c r="D6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E6" t="s">
+        <v>323</v>
+      </c>
+      <c r="F6" t="s">
         <v>325</v>
-      </c>
-      <c r="F6" t="s">
-        <v>327</v>
       </c>
       <c r="G6" t="s">
         <v>132</v>
       </c>
       <c r="H6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I6" t="s">
         <v>134</v>

</xml_diff>